<commit_message>
Updates for DMsan scenario analysis
</commit_message>
<xml_diff>
--- a/dmsan/reclaimer/scores/other_indicator_scores.xlsx
+++ b/dmsan/reclaimer/scores/other_indicator_scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlohm\Dropbox\Lohman-Guest_Shared\12_PhD_Paper3_Sanitation_Decision-Making\Python Code\GitHubDesktop\DMsan\dmsan\reclaimer\scores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A07977E-AD3D-4E1E-A3BE-24913349A585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE75F441-E16F-4AA3-9644-ACB060BB5294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="13" xr2:uid="{672D30C3-4BC8-BB41-BA04-8F7D3B55B551}"/>
+    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15840" firstSheet="13" activeTab="20" xr2:uid="{672D30C3-4BC8-BB41-BA04-8F7D3B55B551}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSummary" sheetId="25" r:id="rId1"/>
@@ -21,11 +21,11 @@
     <sheet name="construction_skills" sheetId="6" r:id="rId6"/>
     <sheet name="OM_complexity" sheetId="7" r:id="rId7"/>
     <sheet name="pop_flexibility" sheetId="8" r:id="rId8"/>
-    <sheet name="electricity_flexibility" sheetId="10" r:id="rId9"/>
-    <sheet name="drought_flexibility" sheetId="11" r:id="rId10"/>
-    <sheet name="water_reuse" sheetId="29" r:id="rId11"/>
-    <sheet name="supply_chain" sheetId="34" r:id="rId12"/>
-    <sheet name="design_job_creation" sheetId="14" r:id="rId13"/>
+    <sheet name="design_job_creation" sheetId="14" r:id="rId9"/>
+    <sheet name="electricity_flexibility" sheetId="10" r:id="rId10"/>
+    <sheet name="drought_flexibility" sheetId="11" r:id="rId11"/>
+    <sheet name="water_reuse" sheetId="29" r:id="rId12"/>
+    <sheet name="supply_chain" sheetId="34" r:id="rId13"/>
     <sheet name="design_high_pay_jobs" sheetId="15" r:id="rId14"/>
     <sheet name="end_user_disposal" sheetId="16" r:id="rId15"/>
     <sheet name="end_user_cleaning" sheetId="17" r:id="rId16"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="181">
   <si>
     <t>Criteria</t>
   </si>
@@ -158,69 +158,21 @@
     <t>End-user acceptability</t>
   </si>
   <si>
-    <t>the conveinence of disposal</t>
-  </si>
-  <si>
-    <t>end_user_disposal_1</t>
-  </si>
-  <si>
     <t>disposal times per year</t>
   </si>
   <si>
-    <t>end_user_disposal_2</t>
-  </si>
-  <si>
-    <t>end_user_disposal_3</t>
-  </si>
-  <si>
     <t>the cleaning requirement for the end user</t>
   </si>
   <si>
-    <t>end_user_cleaning_1</t>
-  </si>
-  <si>
-    <t>end_user_cleaning_2</t>
-  </si>
-  <si>
-    <t>end_user_cleaning_3</t>
-  </si>
-  <si>
     <t>privacy of using the system for the end-user</t>
   </si>
   <si>
-    <t>privacy_1</t>
-  </si>
-  <si>
     <t>households/unit</t>
   </si>
   <si>
-    <t>privacy_2</t>
-  </si>
-  <si>
-    <t>privacy_3</t>
-  </si>
-  <si>
     <t>odor and flies produced by the system</t>
   </si>
   <si>
-    <t>odor_1</t>
-  </si>
-  <si>
-    <t>odor_2</t>
-  </si>
-  <si>
-    <t>odor_3</t>
-  </si>
-  <si>
-    <t>end_user_disposal_safety_1</t>
-  </si>
-  <si>
-    <t>end_user_disposal_safety_2</t>
-  </si>
-  <si>
-    <t>end_user_disposal_safety_3</t>
-  </si>
-  <si>
     <t>security</t>
   </si>
   <si>
@@ -281,24 +233,6 @@
     <t>The convenience of disposal for the management/landlord</t>
   </si>
   <si>
-    <t>management_disposal_1</t>
-  </si>
-  <si>
-    <t>management_disposal_2</t>
-  </si>
-  <si>
-    <t>management_disposal_3</t>
-  </si>
-  <si>
-    <t>management_cleaning_1</t>
-  </si>
-  <si>
-    <t>management_cleaning_2</t>
-  </si>
-  <si>
-    <t>management_cleaning_3</t>
-  </si>
-  <si>
     <t>The cleaning requirement for the management/landlord</t>
   </si>
   <si>
@@ -533,18 +467,6 @@
     <t>Reclaimer C</t>
   </si>
   <si>
-    <t>BiogenicRefinery A</t>
-  </si>
-  <si>
-    <t>BiogenicRefinery B</t>
-  </si>
-  <si>
-    <t>NEWgenerator A</t>
-  </si>
-  <si>
-    <t>NEWgenerator B</t>
-  </si>
-  <si>
     <t>Use in Study</t>
   </si>
   <si>
@@ -629,61 +551,40 @@
     <t>design_high_pay_jobs_6</t>
   </si>
   <si>
-    <t>end_user_disposal_4</t>
-  </si>
-  <si>
     <t>end_user_disposal_5</t>
   </si>
   <si>
     <t>end_user_disposal_6</t>
   </si>
   <si>
-    <t>end_user_cleaning_4</t>
-  </si>
-  <si>
     <t>end_user_cleaning_5</t>
   </si>
   <si>
     <t>end_user_cleaning_6</t>
   </si>
   <si>
-    <t>privacy_4</t>
-  </si>
-  <si>
     <t>privacy_5</t>
   </si>
   <si>
     <t>privacy_6</t>
   </si>
   <si>
-    <t>odor_4</t>
-  </si>
-  <si>
     <t>odor_5</t>
   </si>
   <si>
     <t>odor_6</t>
   </si>
   <si>
-    <t>end_user_disposal_safety_4</t>
-  </si>
-  <si>
     <t>end_user_disposal_safety_5</t>
   </si>
   <si>
     <t>end_user_disposal_safety_6</t>
   </si>
   <si>
-    <t>management_disposal_4</t>
-  </si>
-  <si>
     <t>management_disposal_5</t>
   </si>
   <si>
     <t>management_disposal_6</t>
-  </si>
-  <si>
-    <t>management_cleaning_4</t>
   </si>
   <si>
     <t>management_cleaning_5</t>
@@ -1161,7 +1062,7 @@
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.5" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.5" style="13" bestFit="1" customWidth="1"/>
@@ -1174,41 +1075,41 @@
     <col min="9" max="16384" width="8.6640625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -1223,15 +1124,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:8" s="2" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -1246,18 +1147,18 @@
         <v>12</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -1272,18 +1173,18 @@
         <v>12</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="2" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
@@ -1298,18 +1199,18 @@
         <v>12</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
@@ -1324,18 +1225,18 @@
         <v>12</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
@@ -1350,18 +1251,18 @@
         <v>12</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="3" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>6</v>
@@ -1376,18 +1277,18 @@
         <v>12</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>6</v>
@@ -1402,18 +1303,18 @@
         <v>12</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="3" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>6</v>
@@ -1428,154 +1329,154 @@
         <v>12</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="10" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="10" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>12</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="10" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="10" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="10" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="10" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="10" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="10" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="10" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="10" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="10" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="10" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>10</v>
@@ -1584,18 +1485,18 @@
         <v>12</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>23</v>
@@ -1604,24 +1505,24 @@
         <v>24</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="5" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>23</v>
@@ -1630,24 +1531,24 @@
         <v>24</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="5" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>23</v>
@@ -1656,50 +1557,50 @@
         <v>24</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="6" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="6" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="7" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="7" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>27</v>
@@ -1714,18 +1615,18 @@
         <v>12</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="7" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="7" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>27</v>
@@ -1740,47 +1641,47 @@
         <v>12</v>
       </c>
       <c r="H22" s="19" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="8" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="7" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:8" s="7" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>10</v>
@@ -1790,44 +1691,44 @@
       </c>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:8" s="8" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:8" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="8" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:8" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>10</v>
@@ -1836,21 +1737,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="8" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:8" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>10</v>
@@ -1859,45 +1760,45 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="9" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:8" s="9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>12</v>
       </c>
       <c r="H28" s="19"/>
     </row>
-    <row r="29" spans="1:8" s="9" customFormat="1" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:8" s="9" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>100</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>122</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>10</v>
@@ -1907,7 +1808,7 @@
       </c>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" spans="1:8" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="H30" s="13"/>
     </row>
   </sheetData>
@@ -1918,6 +1819,116 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65B6589-CCE9-E840-BD14-4101024F6783}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.58203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D42364C5-9A17-1840-801C-E3F8B85A8FA6}">
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
@@ -1928,7 +1939,7 @@
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.58203125" bestFit="1" customWidth="1"/>
@@ -1937,18 +1948,18 @@
     <col min="5" max="5" width="18.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -1969,9 +1980,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -1983,7 +1994,7 @@
         <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -1995,9 +2006,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -2009,7 +2020,7 @@
         <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>182</v>
+        <v>156</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -2027,7 +2038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73FC7374-1BFE-4047-B173-DE11D9D2DE36}">
   <sheetPr>
     <tabColor theme="2" tint="0.39997558519241921"/>
@@ -2038,7 +2049,7 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
@@ -2047,18 +2058,18 @@
     <col min="5" max="5" width="13.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -2079,24 +2090,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="E2" t="s">
-        <v>183</v>
+        <v>157</v>
       </c>
       <c r="F2" t="s">
-        <v>213</v>
+        <v>180</v>
       </c>
       <c r="G2">
         <v>720</v>
@@ -2105,24 +2116,24 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="E3" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="F3" t="s">
-        <v>213</v>
+        <v>180</v>
       </c>
       <c r="G3">
         <v>720</v>
@@ -2137,7 +2148,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3730C0-374F-4FC5-B70C-7EA120C190D0}">
   <sheetPr>
     <tabColor theme="2" tint="0.39997558519241921"/>
@@ -2148,7 +2159,7 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
@@ -2157,18 +2168,18 @@
     <col min="5" max="5" width="13.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -2189,24 +2200,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="E2" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
       <c r="F2" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -2215,134 +2226,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="E3" t="s">
-        <v>186</v>
+        <v>160</v>
       </c>
       <c r="F3" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="G3">
         <v>0</v>
-      </c>
-      <c r="J3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00726486-B842-2041-98FE-2E8568208BFC}">
-  <dimension ref="A1:J3"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
-  <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.58203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.08203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.75" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
-        <v>188</v>
-      </c>
-      <c r="F3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
       </c>
       <c r="J3" t="s">
         <v>12</v>
@@ -2358,11 +2262,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E852E00B-F08F-4441-9F51-5EFD877FF5B7}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.58203125" bestFit="1" customWidth="1"/>
@@ -2371,18 +2275,18 @@
     <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -2403,9 +2307,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -2417,7 +2321,7 @@
         <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
       <c r="F2" t="s">
         <v>32</v>
@@ -2429,9 +2333,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
@@ -2443,7 +2347,7 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>190</v>
+        <v>164</v>
       </c>
       <c r="F3" t="s">
         <v>32</v>
@@ -2463,13 +2367,13 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5107C111-3804-1240-99DA-17B1CE3A7796}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.58203125" bestFit="1" customWidth="1"/>
@@ -2479,18 +2383,18 @@
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -2511,9 +2415,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -2522,13 +2426,13 @@
         <v>33</v>
       </c>
       <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2" t="s">
         <v>34</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
-        <v>36</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -2537,9 +2441,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
@@ -2551,119 +2455,15 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>166</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" t="s">
-        <v>191</v>
-      </c>
-      <c r="F5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>192</v>
-      </c>
-      <c r="F6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A7" t="s">
-        <v>158</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2676,30 +2476,30 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC106D18-8739-4443-BF99-297A6DF00AC3}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -2720,9 +2520,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -2731,10 +2531,10 @@
         <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>167</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -2746,9 +2546,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
@@ -2757,10 +2557,10 @@
         <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>168</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -2769,110 +2569,6 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s">
-        <v>194</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="s">
-        <v>195</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A7" t="s">
-        <v>158</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" t="s">
-        <v>196</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2884,13 +2580,13 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC079F57-3A5F-6D4C-90B0-82D26B5B99FE}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G7"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.58203125" bestFit="1" customWidth="1"/>
@@ -2900,18 +2596,18 @@
     <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -2932,9 +2628,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -2943,24 +2639,21 @@
         <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>169</v>
       </c>
       <c r="F2" t="s">
-        <v>212</v>
+        <v>179</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
@@ -2969,113 +2662,15 @@
         <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>170</v>
       </c>
       <c r="F3" t="s">
-        <v>212</v>
+        <v>179</v>
       </c>
       <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="J3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" t="s">
-        <v>212</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" t="s">
-        <v>197</v>
-      </c>
-      <c r="F5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" t="s">
-        <v>198</v>
-      </c>
-      <c r="F6" t="s">
-        <v>212</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A7" t="s">
-        <v>158</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" t="s">
-        <v>199</v>
-      </c>
-      <c r="F7" t="s">
-        <v>212</v>
-      </c>
-      <c r="G7">
         <v>0</v>
       </c>
     </row>
@@ -3087,13 +2682,13 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E32E946-C34C-F245-9D79-E6F684B40381}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G7"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.58203125" bestFit="1" customWidth="1"/>
@@ -3101,18 +2696,18 @@
     <col min="4" max="4" width="32.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -3133,9 +2728,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -3144,10 +2739,10 @@
         <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>171</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -3159,9 +2754,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
@@ -3170,10 +2765,10 @@
         <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>172</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -3182,110 +2777,6 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" t="s">
-        <v>200</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" t="s">
-        <v>201</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A7" t="s">
-        <v>158</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" t="s">
-        <v>202</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3297,13 +2788,13 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E172A0A8-D530-E347-B58E-45BBE3162EF9}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G7"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.58203125" bestFit="1" customWidth="1"/>
@@ -3312,18 +2803,18 @@
     <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -3344,21 +2835,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>173</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -3370,21 +2861,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>174</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -3393,110 +2884,6 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" t="s">
-        <v>203</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" t="s">
-        <v>204</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A7" t="s">
-        <v>158</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" t="s">
-        <v>205</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3517,7 +2904,7 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.58203125" bestFit="1" customWidth="1"/>
@@ -3526,18 +2913,18 @@
     <col min="5" max="5" width="19.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -3558,9 +2945,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -3572,7 +2959,7 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -3584,9 +2971,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -3598,7 +2985,7 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -3618,13 +3005,13 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E332F5F-32EC-C046-8FDB-241E5C1F829A}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G7"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.58203125" bestFit="1" customWidth="1"/>
@@ -3634,18 +3021,18 @@
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -3666,24 +3053,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>175</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -3692,133 +3079,29 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>176</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" t="s">
-        <v>206</v>
-      </c>
-      <c r="F5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" t="s">
-        <v>207</v>
-      </c>
-      <c r="F6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A7" t="s">
-        <v>158</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" t="s">
-        <v>208</v>
-      </c>
-      <c r="F7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3830,13 +3113,13 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E922356-1DFC-4726-8591-7B465EEC758C}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.58203125" bestFit="1" customWidth="1"/>
@@ -3845,18 +3128,18 @@
     <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -3877,21 +3160,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>177</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -3903,21 +3186,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>178</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -3926,110 +3209,6 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" t="s">
-        <v>209</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" t="s">
-        <v>210</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.8">
-      <c r="A7" t="s">
-        <v>158</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" t="s">
-        <v>211</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4050,7 +3229,7 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="8.58203125" bestFit="1" customWidth="1"/>
@@ -4059,18 +3238,18 @@
     <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -4091,9 +3270,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -4105,7 +3284,7 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -4117,9 +3296,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -4131,7 +3310,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -4160,7 +3339,7 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.58203125" bestFit="1" customWidth="1"/>
@@ -4169,18 +3348,18 @@
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -4201,9 +3380,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -4215,7 +3394,7 @@
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>143</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -4227,9 +3406,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -4241,7 +3420,7 @@
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>170</v>
+        <v>144</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -4270,7 +3449,7 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.58203125" bestFit="1" customWidth="1"/>
@@ -4279,18 +3458,18 @@
     <col min="5" max="5" width="16.9140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -4311,9 +3490,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -4325,7 +3504,7 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>171</v>
+        <v>145</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -4337,9 +3516,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -4351,7 +3530,7 @@
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -4380,7 +3559,7 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.58203125" bestFit="1" customWidth="1"/>
@@ -4389,18 +3568,18 @@
     <col min="5" max="5" width="19.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -4421,9 +3600,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -4435,7 +3614,7 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -4447,9 +3626,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -4461,7 +3640,7 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -4490,7 +3669,7 @@
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.58203125" bestFit="1" customWidth="1"/>
@@ -4499,18 +3678,18 @@
     <col min="5" max="5" width="12.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -4531,9 +3710,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -4545,7 +3724,7 @@
         <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>175</v>
+        <v>149</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -4557,9 +3736,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -4571,7 +3750,7 @@
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>176</v>
+        <v>150</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -4600,7 +3779,7 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.58203125" bestFit="1" customWidth="1"/>
@@ -4610,18 +3789,18 @@
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -4642,9 +3821,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -4656,7 +3835,7 @@
         <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>177</v>
+        <v>151</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -4668,9 +3847,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -4682,7 +3861,7 @@
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>178</v>
+        <v>152</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -4701,37 +3880,34 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65B6589-CCE9-E840-BD14-4101024F6783}">
-  <sheetPr>
-    <tabColor theme="4" tint="0.39997558519241921"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00726486-B842-2041-98FE-2E8568208BFC}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.58203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.08203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -4752,56 +3928,56 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>151</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>151</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>